<commit_message>
Final summer practice commit
</commit_message>
<xml_diff>
--- a/FeedbackWebsite/FeedbackWebsite/Excel/Source/Event Feedback Form.xlsx
+++ b/FeedbackWebsite/FeedbackWebsite/Excel/Source/Event Feedback Form.xlsx
@@ -330,6 +330,27 @@
     <xf numFmtId="0" fontId="2" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
@@ -341,9 +362,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -366,26 +384,8 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -696,8 +696,8 @@
   </sheetPr>
   <dimension ref="A1:H26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15"/>
@@ -711,108 +711,106 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="26.25" customHeight="1">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="13" t="s">
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="19" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="63.75" customHeight="1">
-      <c r="A2" s="22" t="s">
+      <c r="A2" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="22"/>
-      <c r="C2" s="22"/>
-      <c r="D2" s="22"/>
-      <c r="E2" s="22"/>
-      <c r="F2" s="14"/>
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="20"/>
     </row>
     <row r="3" spans="1:6" ht="30.75" customHeight="1">
-      <c r="A3" s="20" t="s">
+      <c r="A3" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="20"/>
-      <c r="C3" s="20"/>
-      <c r="D3" s="20"/>
-      <c r="E3" s="20"/>
-      <c r="F3" s="14"/>
+      <c r="B3" s="25"/>
+      <c r="C3" s="25"/>
+      <c r="D3" s="25"/>
+      <c r="E3" s="25"/>
+      <c r="F3" s="20"/>
     </row>
     <row r="4" spans="1:6" ht="15.75" customHeight="1">
       <c r="A4" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="24"/>
-      <c r="C4" s="25"/>
-      <c r="D4" s="26"/>
-      <c r="E4" s="23"/>
-      <c r="F4" s="14"/>
+      <c r="B4" s="12"/>
+      <c r="C4" s="13"/>
+      <c r="D4" s="14"/>
+      <c r="E4" s="27"/>
+      <c r="F4" s="20"/>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="24"/>
-      <c r="C5" s="25"/>
-      <c r="D5" s="26"/>
-      <c r="E5" s="23"/>
-      <c r="F5" s="14"/>
+      <c r="B5" s="12"/>
+      <c r="C5" s="13"/>
+      <c r="D5" s="14"/>
+      <c r="E5" s="27"/>
+      <c r="F5" s="20"/>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="24"/>
-      <c r="C6" s="25"/>
-      <c r="D6" s="26"/>
-      <c r="E6" s="23"/>
-      <c r="F6" s="14"/>
+      <c r="B6" s="12"/>
+      <c r="C6" s="13"/>
+      <c r="D6" s="14"/>
+      <c r="E6" s="27"/>
+      <c r="F6" s="20"/>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="24"/>
-      <c r="C7" s="25"/>
-      <c r="D7" s="26"/>
-      <c r="E7" s="23"/>
-      <c r="F7" s="14"/>
+      <c r="B7" s="12"/>
+      <c r="C7" s="13"/>
+      <c r="D7" s="14"/>
+      <c r="E7" s="27"/>
+      <c r="F7" s="20"/>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="24"/>
-      <c r="C8" s="25"/>
-      <c r="D8" s="26"/>
-      <c r="E8" s="23"/>
-      <c r="F8" s="14"/>
+      <c r="B8" s="12"/>
+      <c r="C8" s="13"/>
+      <c r="D8" s="14"/>
+      <c r="E8" s="27"/>
+      <c r="F8" s="20"/>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B9" s="24"/>
-      <c r="C9" s="25"/>
-      <c r="D9" s="26"/>
-      <c r="E9" s="23"/>
-      <c r="F9" s="14"/>
+      <c r="B9" s="12"/>
+      <c r="C9" s="13"/>
+      <c r="D9" s="14"/>
+      <c r="E9" s="27"/>
+      <c r="F9" s="20"/>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="3">
-        <v>3</v>
-      </c>
+      <c r="B10" s="3"/>
       <c r="C10" s="6"/>
       <c r="D10" s="3"/>
-      <c r="E10" s="23"/>
-      <c r="F10" s="14"/>
+      <c r="E10" s="27"/>
+      <c r="F10" s="20"/>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" s="4" t="s">
@@ -821,172 +819,162 @@
       <c r="B11" s="3"/>
       <c r="C11" s="6"/>
       <c r="D11" s="3"/>
-      <c r="E11" s="23"/>
-      <c r="F11" s="14"/>
+      <c r="E11" s="27"/>
+      <c r="F11" s="20"/>
     </row>
     <row r="12" spans="1:6" ht="55.5" customHeight="1">
-      <c r="A12" s="20" t="s">
+      <c r="A12" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="B12" s="20"/>
-      <c r="C12" s="20"/>
-      <c r="D12" s="20"/>
-      <c r="E12" s="20"/>
-      <c r="F12" s="14"/>
+      <c r="B12" s="25"/>
+      <c r="C12" s="25"/>
+      <c r="D12" s="25"/>
+      <c r="E12" s="25"/>
+      <c r="F12" s="20"/>
     </row>
     <row r="13" spans="1:6">
-      <c r="A13" s="15"/>
-      <c r="B13" s="15"/>
-      <c r="C13" s="15"/>
-      <c r="D13" s="15"/>
+      <c r="A13" s="16"/>
+      <c r="B13" s="16"/>
+      <c r="C13" s="16"/>
+      <c r="D13" s="16"/>
       <c r="E13" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="F13" s="14"/>
+      <c r="F13" s="20"/>
     </row>
     <row r="14" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A14" s="27" t="s">
+      <c r="A14" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="B14" s="27"/>
-      <c r="C14" s="27"/>
-      <c r="D14" s="27"/>
+      <c r="B14" s="15"/>
+      <c r="C14" s="15"/>
+      <c r="D14" s="15"/>
       <c r="E14" s="7"/>
-      <c r="F14" s="14"/>
+      <c r="F14" s="20"/>
     </row>
     <row r="15" spans="1:6">
-      <c r="A15" s="27" t="s">
+      <c r="A15" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="B15" s="27"/>
-      <c r="C15" s="27"/>
-      <c r="D15" s="27"/>
+      <c r="B15" s="15"/>
+      <c r="C15" s="15"/>
+      <c r="D15" s="15"/>
       <c r="E15" s="7"/>
-      <c r="F15" s="14"/>
+      <c r="F15" s="20"/>
     </row>
     <row r="16" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A16" s="22" t="s">
+      <c r="A16" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="B16" s="22"/>
-      <c r="C16" s="22"/>
-      <c r="D16" s="22"/>
+      <c r="B16" s="11"/>
+      <c r="C16" s="11"/>
+      <c r="D16" s="11"/>
       <c r="E16" s="7"/>
-      <c r="F16" s="14"/>
+      <c r="F16" s="20"/>
     </row>
     <row r="17" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A17" s="22" t="s">
+      <c r="A17" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="B17" s="22"/>
-      <c r="C17" s="22"/>
-      <c r="D17" s="22"/>
+      <c r="B17" s="11"/>
+      <c r="C17" s="11"/>
+      <c r="D17" s="11"/>
       <c r="E17" s="7"/>
-      <c r="F17" s="14"/>
+      <c r="F17" s="20"/>
     </row>
     <row r="18" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A18" s="22" t="s">
+      <c r="A18" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="B18" s="22"/>
-      <c r="C18" s="22"/>
-      <c r="D18" s="22"/>
+      <c r="B18" s="11"/>
+      <c r="C18" s="11"/>
+      <c r="D18" s="11"/>
       <c r="E18" s="7"/>
-      <c r="F18" s="14"/>
+      <c r="F18" s="20"/>
     </row>
     <row r="19" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A19" s="22" t="s">
+      <c r="A19" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="B19" s="22"/>
-      <c r="C19" s="22"/>
-      <c r="D19" s="22"/>
+      <c r="B19" s="11"/>
+      <c r="C19" s="11"/>
+      <c r="D19" s="11"/>
       <c r="E19" s="7"/>
-      <c r="F19" s="14"/>
+      <c r="F19" s="20"/>
     </row>
     <row r="20" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A20" s="22" t="s">
+      <c r="A20" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="B20" s="22"/>
-      <c r="C20" s="22"/>
-      <c r="D20" s="22"/>
+      <c r="B20" s="11"/>
+      <c r="C20" s="11"/>
+      <c r="D20" s="11"/>
       <c r="E20" s="7"/>
-      <c r="F20" s="14"/>
+      <c r="F20" s="20"/>
     </row>
     <row r="21" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A21" s="22" t="s">
+      <c r="A21" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="B21" s="22"/>
-      <c r="C21" s="22"/>
-      <c r="D21" s="22"/>
+      <c r="B21" s="11"/>
+      <c r="C21" s="11"/>
+      <c r="D21" s="11"/>
       <c r="E21" s="7"/>
-      <c r="F21" s="14"/>
+      <c r="F21" s="20"/>
     </row>
     <row r="22" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A22" s="22" t="s">
+      <c r="A22" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="B22" s="22"/>
-      <c r="C22" s="22"/>
-      <c r="D22" s="22"/>
+      <c r="B22" s="11"/>
+      <c r="C22" s="11"/>
+      <c r="D22" s="11"/>
       <c r="E22" s="7"/>
-      <c r="F22" s="14"/>
+      <c r="F22" s="20"/>
     </row>
     <row r="23" spans="1:8">
-      <c r="A23" s="15"/>
-      <c r="B23" s="15"/>
-      <c r="C23" s="15"/>
-      <c r="D23" s="15"/>
-      <c r="E23" s="15"/>
-      <c r="F23" s="14"/>
+      <c r="A23" s="16"/>
+      <c r="B23" s="16"/>
+      <c r="C23" s="16"/>
+      <c r="D23" s="16"/>
+      <c r="E23" s="16"/>
+      <c r="F23" s="20"/>
     </row>
     <row r="24" spans="1:8" ht="30" customHeight="1">
-      <c r="A24" s="16" t="s">
+      <c r="A24" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="B24" s="16"/>
-      <c r="C24" s="16"/>
-      <c r="D24" s="16"/>
-      <c r="E24" s="16"/>
-      <c r="F24" s="14"/>
+      <c r="B24" s="21"/>
+      <c r="C24" s="21"/>
+      <c r="D24" s="21"/>
+      <c r="E24" s="21"/>
+      <c r="F24" s="20"/>
       <c r="G24" s="9"/>
       <c r="H24" s="8"/>
     </row>
     <row r="25" spans="1:8" s="2" customFormat="1" ht="83.25" customHeight="1">
-      <c r="A25" s="17"/>
-      <c r="B25" s="18"/>
-      <c r="C25" s="18"/>
-      <c r="D25" s="18"/>
-      <c r="E25" s="19"/>
-      <c r="F25" s="14"/>
+      <c r="A25" s="22"/>
+      <c r="B25" s="23"/>
+      <c r="C25" s="23"/>
+      <c r="D25" s="23"/>
+      <c r="E25" s="24"/>
+      <c r="F25" s="20"/>
       <c r="G25" s="10"/>
       <c r="H25" s="8"/>
     </row>
     <row r="26" spans="1:8" ht="15.6">
-      <c r="A26" s="11"/>
-      <c r="B26" s="12"/>
-      <c r="C26" s="12"/>
-      <c r="D26" s="12"/>
-      <c r="E26" s="12"/>
-      <c r="F26" s="14"/>
+      <c r="A26" s="17"/>
+      <c r="B26" s="18"/>
+      <c r="C26" s="18"/>
+      <c r="D26" s="18"/>
+      <c r="E26" s="18"/>
+      <c r="F26" s="20"/>
       <c r="G26" s="8"/>
       <c r="H26" s="8"/>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1"/>
   <mergeCells count="26">
-    <mergeCell ref="A20:D20"/>
-    <mergeCell ref="A21:D21"/>
-    <mergeCell ref="A22:D22"/>
-    <mergeCell ref="A16:D16"/>
-    <mergeCell ref="A17:D17"/>
-    <mergeCell ref="B6:D6"/>
-    <mergeCell ref="B7:D7"/>
-    <mergeCell ref="A15:D15"/>
-    <mergeCell ref="A13:D13"/>
-    <mergeCell ref="A14:D14"/>
     <mergeCell ref="A26:E26"/>
     <mergeCell ref="F1:F26"/>
     <mergeCell ref="A23:E23"/>
@@ -1003,6 +991,16 @@
     <mergeCell ref="B9:D9"/>
     <mergeCell ref="A19:D19"/>
     <mergeCell ref="B5:D5"/>
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="A15:D15"/>
+    <mergeCell ref="A13:D13"/>
+    <mergeCell ref="A14:D14"/>
+    <mergeCell ref="A20:D20"/>
+    <mergeCell ref="A21:D21"/>
+    <mergeCell ref="A22:D22"/>
+    <mergeCell ref="A16:D16"/>
+    <mergeCell ref="A17:D17"/>
   </mergeCells>
   <dataValidations count="12">
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Type your comment here" sqref="A25"/>

</xml_diff>